<commit_message>
opdateret bilag. Mangler burndown timer + user stories
</commit_message>
<xml_diff>
--- a/BurndownCharts/Burndowns.xlsx
+++ b/BurndownCharts/Burndowns.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="2"/>
@@ -184,12 +184,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -197,6 +191,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -307,11 +307,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69689728"/>
-        <c:axId val="69691264"/>
+        <c:axId val="115713536"/>
+        <c:axId val="115715072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69689728"/>
+        <c:axId val="115713536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -320,7 +320,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69691264"/>
+        <c:crossAx val="115715072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -328,7 +328,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69691264"/>
+        <c:axId val="115715072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -339,7 +339,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69689728"/>
+        <c:crossAx val="115713536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -455,11 +455,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190669184"/>
-        <c:axId val="190670720"/>
+        <c:axId val="116637696"/>
+        <c:axId val="116639232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190669184"/>
+        <c:axId val="116637696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -468,7 +468,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190670720"/>
+        <c:crossAx val="116639232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -476,7 +476,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190670720"/>
+        <c:axId val="116639232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,7 +487,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190669184"/>
+        <c:crossAx val="116637696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -532,6 +532,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Brændt</c:v>
+          </c:tx>
           <c:val>
             <c:numRef>
               <c:f>'Iteration 3'!$B$3:$B$5</c:f>
@@ -555,6 +558,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Planlagt</c:v>
+          </c:tx>
           <c:val>
             <c:numRef>
               <c:f>'Iteration 3'!$C$3:$C$5</c:f>
@@ -585,11 +591,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="167380864"/>
-        <c:axId val="167382400"/>
+        <c:axId val="116336896"/>
+        <c:axId val="116359168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="167380864"/>
+        <c:axId val="116336896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -598,7 +604,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167382400"/>
+        <c:crossAx val="116359168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -606,7 +612,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="167382400"/>
+        <c:axId val="116359168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -617,7 +623,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167380864"/>
+        <c:crossAx val="116336896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -643,16 +649,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123824</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1035,15 +1041,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A9" sqref="A9:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1058,7 +1064,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1068,15 +1074,8 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="6"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1086,15 +1085,8 @@
       <c r="C3">
         <v>12.5</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1104,15 +1096,8 @@
       <c r="C4">
         <v>9.375</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1123,7 +1108,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1134,7 +1119,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1144,13 +1129,41 @@
       <c r="C7">
         <v>0</v>
       </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1162,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P3" sqref="P3:T3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,13 +1206,13 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="6"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1211,13 +1224,13 @@
       <c r="C3">
         <v>20</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1229,13 +1242,13 @@
       <c r="C4">
         <v>15</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1288,7 +1301,7 @@
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="P2" sqref="P2:T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,13 +1331,13 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="6"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1336,13 +1349,13 @@
       <c r="C3">
         <v>11</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1354,13 +1367,13 @@
       <c r="C4">
         <v>5.5</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">

</xml_diff>